<commit_message>
Added user stories to sprint log
</commit_message>
<xml_diff>
--- a/Breadbox Sprint Backlog.xlsx
+++ b/Breadbox Sprint Backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="50">
   <si>
     <t>Effort Remaining</t>
   </si>
@@ -75,6 +75,10 @@
     <t>Accessibility features</t>
   </si>
   <si>
+    <t xml:space="preserve">As a user, I want to be able to change the features of the website to make it easier to interact with. I want to be able to change the colours of the text and the background so that it's easier to read, I want to make the text bigger and the fonts clearer. 
+As a develepor, I want to make sure my product meets the accessability requirements for websites so we can attract more users and keep them. </t>
+  </si>
+  <si>
     <t>Scaling Back</t>
   </si>
   <si>
@@ -93,6 +97,10 @@
     <t>Implement user profiles</t>
   </si>
   <si>
+    <t xml:space="preserve">As a user i want to be able to create an account without using an email address so nobody knows it's me.
+</t>
+  </si>
+  <si>
     <t>Ryan</t>
   </si>
   <si>
@@ -106,6 +114,10 @@
   </si>
   <si>
     <t>Emergency support page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a user, I want a page that I can go to for times when I feel I need help quickly. I also feel this page should have many options for help so I don't need to go searching the website. 
+As a developer, I want to make sure that the emergency support page is filled with content that would help an individual who is in need of quick help. </t>
   </si>
   <si>
     <t>Comepleted</t>
@@ -126,6 +138,10 @@
     <t>Security checks</t>
   </si>
   <si>
+    <t>as a user i want my information to be secure
+as a developer i want it to be safe for users and meet security standards</t>
+  </si>
+  <si>
     <t>Wells &amp; Emmanuel</t>
   </si>
   <si>
@@ -139,6 +155,10 @@
   </si>
   <si>
     <t>User Preferences</t>
+  </si>
+  <si>
+    <t>as a user i want to be able to have my prefrences saved to my account when i log in
+as a developer I want to be able to have the CSS changes securely saved for each account</t>
   </si>
   <si>
     <t>Jack</t>
@@ -313,7 +333,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -336,7 +356,7 @@
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
@@ -368,7 +388,7 @@
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
@@ -395,13 +415,10 @@
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="4" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="4" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
@@ -728,15 +745,17 @@
       <c r="B3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="7"/>
+      <c r="C3" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="D3" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G3" s="11">
         <v>5.0</v>
@@ -786,13 +805,13 @@
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
       <c r="D4" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="10" t="s">
         <v>22</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>21</v>
       </c>
       <c r="G4" s="11">
         <v>5.0</v>
@@ -837,18 +856,18 @@
       <c r="Y4" s="3"/>
       <c r="Z4" s="3"/>
     </row>
-    <row r="5" ht="37.5" customHeight="1">
+    <row r="5" ht="123.75" customHeight="1">
       <c r="A5" s="13"/>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
       <c r="D5" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G5" s="17">
         <v>5.0</v>
@@ -898,17 +917,19 @@
         <v>1.0</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="19"/>
+        <v>25</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>26</v>
+      </c>
       <c r="D6" s="20" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G6" s="23">
         <v>5.0</v>
@@ -958,13 +979,13 @@
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
       <c r="D7" s="24" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E7" s="25" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F7" s="26" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G7" s="18">
         <v>10.0</v>
@@ -1014,13 +1035,13 @@
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
       <c r="D8" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="26" t="s">
         <v>27</v>
-      </c>
-      <c r="E8" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="26" t="s">
-        <v>25</v>
       </c>
       <c r="G8" s="12"/>
       <c r="H8" s="11">
@@ -1068,13 +1089,13 @@
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
       <c r="D9" s="24" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F9" s="26" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G9" s="13"/>
       <c r="H9" s="11">
@@ -1117,22 +1138,24 @@
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
     </row>
-    <row r="10" ht="37.5" customHeight="1">
+    <row r="10" ht="53.25" customHeight="1">
       <c r="A10" s="6">
         <v>3.0</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="28"/>
+        <v>31</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>32</v>
+      </c>
       <c r="D10" s="24" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F10" s="29" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G10" s="6">
         <v>5.0</v>
@@ -1177,18 +1200,18 @@
       <c r="Y10" s="3"/>
       <c r="Z10" s="3"/>
     </row>
-    <row r="11" ht="37.5" customHeight="1">
+    <row r="11" ht="53.25" customHeight="1">
       <c r="A11" s="12"/>
       <c r="B11" s="12"/>
       <c r="C11" s="12"/>
       <c r="D11" s="8" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F11" s="29" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G11" s="12"/>
       <c r="H11" s="11">
@@ -1231,18 +1254,18 @@
       <c r="Y11" s="3"/>
       <c r="Z11" s="3"/>
     </row>
-    <row r="12" ht="37.5" customHeight="1">
+    <row r="12" ht="53.25" customHeight="1">
       <c r="A12" s="12"/>
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
       <c r="D12" s="8" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E12" s="25" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F12" s="29" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G12" s="12"/>
       <c r="H12" s="11">
@@ -1285,18 +1308,18 @@
       <c r="Y12" s="3"/>
       <c r="Z12" s="3"/>
     </row>
-    <row r="13" ht="37.5" customHeight="1">
+    <row r="13" ht="53.25" customHeight="1">
       <c r="A13" s="13"/>
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
       <c r="D13" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="29" t="s">
         <v>34</v>
-      </c>
-      <c r="E13" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="F13" s="29" t="s">
-        <v>31</v>
       </c>
       <c r="G13" s="13"/>
       <c r="H13" s="11">
@@ -1344,17 +1367,19 @@
         <v>5.0</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="30"/>
+        <v>38</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>39</v>
+      </c>
       <c r="D14" s="24" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E14" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14" s="31" t="s">
-        <v>36</v>
+        <v>21</v>
+      </c>
+      <c r="F14" s="30" t="s">
+        <v>40</v>
       </c>
       <c r="G14" s="6">
         <v>5.0</v>
@@ -1404,13 +1429,13 @@
       <c r="B15" s="12"/>
       <c r="C15" s="12"/>
       <c r="D15" s="24" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E15" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" s="31" t="s">
-        <v>36</v>
+        <v>21</v>
+      </c>
+      <c r="F15" s="30" t="s">
+        <v>40</v>
       </c>
       <c r="G15" s="12"/>
       <c r="H15" s="11">
@@ -1458,13 +1483,13 @@
       <c r="B16" s="12"/>
       <c r="C16" s="12"/>
       <c r="D16" s="24" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E16" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="F16" s="31" t="s">
-        <v>36</v>
+        <v>21</v>
+      </c>
+      <c r="F16" s="30" t="s">
+        <v>40</v>
       </c>
       <c r="G16" s="12"/>
       <c r="H16" s="11">
@@ -1512,13 +1537,13 @@
       <c r="B17" s="12"/>
       <c r="C17" s="12"/>
       <c r="D17" s="8" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E17" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="F17" s="31" t="s">
-        <v>36</v>
+        <v>21</v>
+      </c>
+      <c r="F17" s="30" t="s">
+        <v>40</v>
       </c>
       <c r="G17" s="12"/>
       <c r="H17" s="11">
@@ -1566,13 +1591,13 @@
       <c r="B18" s="13"/>
       <c r="C18" s="13"/>
       <c r="D18" s="8" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E18" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="F18" s="31" t="s">
-        <v>36</v>
+        <v>21</v>
+      </c>
+      <c r="F18" s="30" t="s">
+        <v>40</v>
       </c>
       <c r="G18" s="13"/>
       <c r="H18" s="11">
@@ -1620,17 +1645,19 @@
         <v>8.0</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="30"/>
+        <v>44</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>45</v>
+      </c>
       <c r="D19" s="24" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E19" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="F19" s="32" t="s">
-        <v>41</v>
+        <v>21</v>
+      </c>
+      <c r="F19" s="31" t="s">
+        <v>46</v>
       </c>
       <c r="G19" s="6">
         <v>5.0</v>
@@ -1679,14 +1706,14 @@
       <c r="A20" s="12"/>
       <c r="B20" s="12"/>
       <c r="C20" s="12"/>
-      <c r="D20" s="33" t="s">
-        <v>42</v>
+      <c r="D20" s="32" t="s">
+        <v>47</v>
       </c>
       <c r="E20" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="F20" s="32" t="s">
-        <v>41</v>
+        <v>21</v>
+      </c>
+      <c r="F20" s="31" t="s">
+        <v>46</v>
       </c>
       <c r="G20" s="12"/>
       <c r="H20" s="11">
@@ -1733,14 +1760,14 @@
       <c r="A21" s="12"/>
       <c r="B21" s="12"/>
       <c r="C21" s="12"/>
-      <c r="D21" s="33" t="s">
-        <v>43</v>
+      <c r="D21" s="32" t="s">
+        <v>48</v>
       </c>
       <c r="E21" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="F21" s="32" t="s">
-        <v>41</v>
+        <v>21</v>
+      </c>
+      <c r="F21" s="31" t="s">
+        <v>46</v>
       </c>
       <c r="G21" s="12"/>
       <c r="H21" s="11">
@@ -1788,13 +1815,13 @@
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
       <c r="D22" s="11" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="E22" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="F22" s="32" t="s">
-        <v>41</v>
+        <v>21</v>
+      </c>
+      <c r="F22" s="31" t="s">
+        <v>46</v>
       </c>
       <c r="G22" s="12"/>
       <c r="H22" s="11">
@@ -1842,13 +1869,13 @@
       <c r="B23" s="13"/>
       <c r="C23" s="13"/>
       <c r="D23" s="11" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E23" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="F23" s="32" t="s">
-        <v>41</v>
+        <v>21</v>
+      </c>
+      <c r="F23" s="31" t="s">
+        <v>46</v>
       </c>
       <c r="G23" s="13"/>
       <c r="H23" s="11">

</xml_diff>